<commit_message>
feat: add mirador link
</commit_message>
<xml_diff>
--- a/docs/iiif/metadata/nishikie.xlsx
+++ b/docs/iiif/metadata/nishikie.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,6 +427,11 @@
           <t>Title</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -434,6 +439,11 @@
           <t>東京大学史料編纂所</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://hi-viewer.web.app/mirador/?manifest=https://hi-ut.github.io/dataset/iiif/collection/nishikie_hi.json</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -441,11 +451,21 @@
           <t>静岡県立中央図書館</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://hi-viewer.web.app/mirador/?manifest=https://hi-ut.github.io/dataset/iiif/collection/nishikie_shizuoka.json</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
           <t>横浜開港資料館</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://hi-viewer.web.app/mirador/?manifest=https://hi-ut.github.io/dataset/iiif/collection/nishikie_yokohama.json</t>
         </is>
       </c>
     </row>

</xml_diff>